<commit_message>
Updated few shot results.
</commit_message>
<xml_diff>
--- a/results/few_shot.xlsx
+++ b/results/few_shot.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ddesblancs/Documents/zeroNoteSamba/results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E95ACE68-74C6-2A45-8214-24773FDE789C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B84C867-AE96-1141-B745-C4DC50DADDDA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5740" yWindow="500" windowWidth="23060" windowHeight="16020" xr2:uid="{6D97F020-2EF7-D34C-8569-EFB580207884}"/>
+    <workbookView xWindow="14100" yWindow="500" windowWidth="14700" windowHeight="16020" xr2:uid="{6D97F020-2EF7-D34C-8569-EFB580207884}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2344" uniqueCount="623">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2452" uniqueCount="643">
   <si>
     <t>Dataset</t>
   </si>
@@ -1901,6 +1901,66 @@
   </si>
   <si>
     <t>0.416</t>
+  </si>
+  <si>
+    <t>0.670</t>
+  </si>
+  <si>
+    <t>0.767</t>
+  </si>
+  <si>
+    <t>0.630</t>
+  </si>
+  <si>
+    <t>0.691</t>
+  </si>
+  <si>
+    <t>0.580</t>
+  </si>
+  <si>
+    <t>0.601</t>
+  </si>
+  <si>
+    <t>0.635</t>
+  </si>
+  <si>
+    <t>0.737</t>
+  </si>
+  <si>
+    <t>0.525</t>
+  </si>
+  <si>
+    <t>0.778</t>
+  </si>
+  <si>
+    <t>0.438</t>
+  </si>
+  <si>
+    <t>0.586</t>
+  </si>
+  <si>
+    <t>0.477</t>
+  </si>
+  <si>
+    <t>0.697</t>
+  </si>
+  <si>
+    <t>0.827</t>
+  </si>
+  <si>
+    <t>0.854</t>
+  </si>
+  <si>
+    <t>0.466</t>
+  </si>
+  <si>
+    <t>0.437</t>
+  </si>
+  <si>
+    <t>0.533</t>
+  </si>
+  <si>
+    <t>0.548</t>
   </si>
 </sst>
 </file>
@@ -2347,8 +2407,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F388871D-55E8-4541-BACB-557B28719449}">
   <dimension ref="A1:W145"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="I61" sqref="I61"/>
+    <sheetView tabSelected="1" topLeftCell="J110" workbookViewId="0">
+      <selection activeCell="R133" sqref="R133"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5036,10 +5096,18 @@
       <c r="M50" s="14" t="s">
         <v>404</v>
       </c>
-      <c r="N50" s="15"/>
-      <c r="O50" s="14"/>
-      <c r="P50" s="14"/>
-      <c r="Q50" s="14"/>
+      <c r="N50" s="15" t="s">
+        <v>376</v>
+      </c>
+      <c r="O50" s="14" t="s">
+        <v>630</v>
+      </c>
+      <c r="P50" s="14" t="s">
+        <v>296</v>
+      </c>
+      <c r="Q50" s="14" t="s">
+        <v>366</v>
+      </c>
       <c r="R50" s="9"/>
       <c r="S50" s="7"/>
       <c r="T50" s="7"/>
@@ -5087,10 +5155,18 @@
       <c r="M51" s="14" t="s">
         <v>297</v>
       </c>
-      <c r="N51" s="15"/>
-      <c r="O51" s="14"/>
-      <c r="P51" s="14"/>
-      <c r="Q51" s="14"/>
+      <c r="N51" s="15" t="s">
+        <v>111</v>
+      </c>
+      <c r="O51" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="P51" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q51" s="14" t="s">
+        <v>25</v>
+      </c>
       <c r="R51" s="9"/>
       <c r="S51" s="7"/>
       <c r="T51" s="7"/>
@@ -5138,10 +5214,18 @@
       <c r="M52" s="14" t="s">
         <v>614</v>
       </c>
-      <c r="N52" s="15"/>
-      <c r="O52" s="14"/>
-      <c r="P52" s="14"/>
-      <c r="Q52" s="14"/>
+      <c r="N52" s="15" t="s">
+        <v>541</v>
+      </c>
+      <c r="O52" s="14" t="s">
+        <v>271</v>
+      </c>
+      <c r="P52" s="14" t="s">
+        <v>634</v>
+      </c>
+      <c r="Q52" s="14" t="s">
+        <v>514</v>
+      </c>
       <c r="R52" s="9"/>
       <c r="S52" s="6"/>
       <c r="T52" s="6"/>
@@ -5189,10 +5273,18 @@
       <c r="M53" s="14" t="s">
         <v>379</v>
       </c>
-      <c r="N53" s="15"/>
-      <c r="O53" s="14"/>
-      <c r="P53" s="14"/>
-      <c r="Q53" s="14"/>
+      <c r="N53" s="15" t="s">
+        <v>574</v>
+      </c>
+      <c r="O53" s="14" t="s">
+        <v>491</v>
+      </c>
+      <c r="P53" s="14" t="s">
+        <v>264</v>
+      </c>
+      <c r="Q53" s="14" t="s">
+        <v>9</v>
+      </c>
       <c r="R53" s="9"/>
       <c r="S53" s="6"/>
       <c r="T53" s="6"/>
@@ -5240,10 +5332,18 @@
       <c r="M54" s="14" t="s">
         <v>133</v>
       </c>
-      <c r="N54" s="15"/>
-      <c r="O54" s="14"/>
-      <c r="P54" s="14"/>
-      <c r="Q54" s="14"/>
+      <c r="N54" s="15" t="s">
+        <v>536</v>
+      </c>
+      <c r="O54" s="14" t="s">
+        <v>631</v>
+      </c>
+      <c r="P54" s="14" t="s">
+        <v>400</v>
+      </c>
+      <c r="Q54" s="14" t="s">
+        <v>636</v>
+      </c>
       <c r="R54" s="9"/>
       <c r="S54" s="7"/>
       <c r="T54" s="7"/>
@@ -5291,10 +5391,18 @@
       <c r="M55" s="14" t="s">
         <v>615</v>
       </c>
-      <c r="N55" s="15"/>
-      <c r="O55" s="14"/>
-      <c r="P55" s="14"/>
-      <c r="Q55" s="14"/>
+      <c r="N55" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="O55" s="14" t="s">
+        <v>559</v>
+      </c>
+      <c r="P55" s="14" t="s">
+        <v>578</v>
+      </c>
+      <c r="Q55" s="14" t="s">
+        <v>9</v>
+      </c>
       <c r="R55" s="9"/>
       <c r="S55" s="7"/>
       <c r="T55" s="7"/>
@@ -5342,10 +5450,18 @@
       <c r="M56" s="15" t="s">
         <v>258</v>
       </c>
-      <c r="N56" s="15"/>
-      <c r="O56" s="15"/>
-      <c r="P56" s="15"/>
-      <c r="Q56" s="15"/>
+      <c r="N56" s="15" t="s">
+        <v>364</v>
+      </c>
+      <c r="O56" s="15" t="s">
+        <v>470</v>
+      </c>
+      <c r="P56" s="15" t="s">
+        <v>632</v>
+      </c>
+      <c r="Q56" s="15" t="s">
+        <v>637</v>
+      </c>
       <c r="R56" s="9"/>
       <c r="S56" s="7"/>
       <c r="T56" s="7"/>
@@ -5393,10 +5509,18 @@
       <c r="M57" s="15" t="s">
         <v>63</v>
       </c>
-      <c r="N57" s="15"/>
-      <c r="O57" s="15"/>
-      <c r="P57" s="15"/>
-      <c r="Q57" s="15"/>
+      <c r="N57" s="15" t="s">
+        <v>101</v>
+      </c>
+      <c r="O57" s="15" t="s">
+        <v>259</v>
+      </c>
+      <c r="P57" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q57" s="15" t="s">
+        <v>28</v>
+      </c>
       <c r="R57" s="9"/>
       <c r="S57" s="7"/>
       <c r="T57" s="7"/>
@@ -5444,10 +5568,18 @@
       <c r="M58" s="15" t="s">
         <v>616</v>
       </c>
-      <c r="N58" s="15"/>
-      <c r="O58" s="14"/>
-      <c r="P58" s="14"/>
-      <c r="Q58" s="14"/>
+      <c r="N58" s="15" t="s">
+        <v>527</v>
+      </c>
+      <c r="O58" s="14" t="s">
+        <v>632</v>
+      </c>
+      <c r="P58" s="14" t="s">
+        <v>428</v>
+      </c>
+      <c r="Q58" s="14" t="s">
+        <v>638</v>
+      </c>
       <c r="R58" s="10"/>
       <c r="S58" s="7"/>
       <c r="T58" s="7"/>
@@ -5495,10 +5627,18 @@
       <c r="M59" s="15" t="s">
         <v>82</v>
       </c>
-      <c r="N59" s="15"/>
-      <c r="O59" s="14"/>
-      <c r="P59" s="14"/>
-      <c r="Q59" s="14"/>
+      <c r="N59" s="15" t="s">
+        <v>277</v>
+      </c>
+      <c r="O59" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="P59" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q59" s="14" t="s">
+        <v>25</v>
+      </c>
       <c r="R59" s="8"/>
       <c r="S59" s="7"/>
       <c r="T59" s="7"/>
@@ -5546,10 +5686,18 @@
       <c r="M60" s="15" t="s">
         <v>161</v>
       </c>
-      <c r="N60" s="15"/>
-      <c r="O60" s="14"/>
-      <c r="P60" s="14"/>
-      <c r="Q60" s="14"/>
+      <c r="N60" s="15" t="s">
+        <v>633</v>
+      </c>
+      <c r="O60" s="14" t="s">
+        <v>487</v>
+      </c>
+      <c r="P60" s="14" t="s">
+        <v>635</v>
+      </c>
+      <c r="Q60" s="14" t="s">
+        <v>233</v>
+      </c>
       <c r="R60" s="9"/>
       <c r="S60" s="7"/>
       <c r="T60" s="7"/>
@@ -5597,10 +5745,18 @@
       <c r="M61" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="N61" s="15"/>
-      <c r="O61" s="14"/>
-      <c r="P61" s="14"/>
-      <c r="Q61" s="14"/>
+      <c r="N61" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="O61" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="P61" s="14" t="s">
+        <v>152</v>
+      </c>
+      <c r="Q61" s="14" t="s">
+        <v>146</v>
+      </c>
       <c r="R61" s="9"/>
       <c r="S61" s="7"/>
       <c r="T61" s="7"/>
@@ -7061,7 +7217,9 @@
       <c r="P86" s="14" t="s">
         <v>605</v>
       </c>
-      <c r="Q86" s="14"/>
+      <c r="Q86" s="14" t="s">
+        <v>400</v>
+      </c>
       <c r="R86" s="7"/>
       <c r="S86" s="9"/>
       <c r="T86" s="9"/>
@@ -7116,7 +7274,9 @@
       <c r="P87" s="14" t="s">
         <v>127</v>
       </c>
-      <c r="Q87" s="14"/>
+      <c r="Q87" s="14" t="s">
+        <v>11</v>
+      </c>
       <c r="R87" s="7"/>
       <c r="S87" s="9"/>
       <c r="T87" s="9"/>
@@ -7171,7 +7331,9 @@
       <c r="P88" s="14" t="s">
         <v>396</v>
       </c>
-      <c r="Q88" s="14"/>
+      <c r="Q88" s="14" t="s">
+        <v>177</v>
+      </c>
       <c r="R88" s="7"/>
       <c r="S88" s="9"/>
       <c r="T88" s="9"/>
@@ -7226,7 +7388,9 @@
       <c r="P89" s="14" t="s">
         <v>578</v>
       </c>
-      <c r="Q89" s="14"/>
+      <c r="Q89" s="14" t="s">
+        <v>17</v>
+      </c>
       <c r="R89" s="11"/>
       <c r="S89" s="9"/>
       <c r="T89" s="9"/>
@@ -7281,7 +7445,9 @@
       <c r="P90" s="14" t="s">
         <v>337</v>
       </c>
-      <c r="Q90" s="14"/>
+      <c r="Q90" s="14" t="s">
+        <v>322</v>
+      </c>
       <c r="R90" s="6"/>
       <c r="S90" s="9"/>
       <c r="T90" s="9"/>
@@ -7336,7 +7502,9 @@
       <c r="P91" s="14" t="s">
         <v>491</v>
       </c>
-      <c r="Q91" s="14"/>
+      <c r="Q91" s="14" t="s">
+        <v>19</v>
+      </c>
       <c r="R91" s="7"/>
       <c r="S91" s="9"/>
       <c r="T91" s="9"/>
@@ -7391,7 +7559,9 @@
       <c r="P92" s="14" t="s">
         <v>413</v>
       </c>
-      <c r="Q92" s="14"/>
+      <c r="Q92" s="14" t="s">
+        <v>623</v>
+      </c>
       <c r="R92" s="7"/>
       <c r="S92" s="9"/>
       <c r="T92" s="9"/>
@@ -7446,7 +7616,9 @@
       <c r="P93" s="15" t="s">
         <v>264</v>
       </c>
-      <c r="Q93" s="14"/>
+      <c r="Q93" s="14" t="s">
+        <v>15</v>
+      </c>
       <c r="R93" s="7"/>
       <c r="S93" s="9"/>
       <c r="T93" s="9"/>
@@ -7501,7 +7673,9 @@
       <c r="P94" s="15" t="s">
         <v>359</v>
       </c>
-      <c r="Q94" s="15"/>
+      <c r="Q94" s="15" t="s">
+        <v>624</v>
+      </c>
       <c r="R94" s="7"/>
       <c r="S94" s="9"/>
       <c r="T94" s="9"/>
@@ -7556,7 +7730,9 @@
       <c r="P95" s="14" t="s">
         <v>578</v>
       </c>
-      <c r="Q95" s="15"/>
+      <c r="Q95" s="15" t="s">
+        <v>114</v>
+      </c>
       <c r="R95" s="7"/>
       <c r="S95" s="9"/>
       <c r="T95" s="9"/>
@@ -7611,7 +7787,9 @@
       <c r="P96" s="14" t="s">
         <v>166</v>
       </c>
-      <c r="Q96" s="14"/>
+      <c r="Q96" s="14" t="s">
+        <v>611</v>
+      </c>
       <c r="R96" s="7"/>
       <c r="S96" s="9"/>
       <c r="T96" s="9"/>
@@ -7666,7 +7844,9 @@
       <c r="P97" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="Q97" s="14"/>
+      <c r="Q97" s="14" t="s">
+        <v>14</v>
+      </c>
       <c r="R97" s="7"/>
       <c r="S97" s="9"/>
       <c r="T97" s="9"/>
@@ -8996,10 +9176,18 @@
       <c r="M122" s="15" t="s">
         <v>193</v>
       </c>
-      <c r="N122" s="14"/>
-      <c r="O122" s="14"/>
-      <c r="P122" s="14"/>
-      <c r="Q122" s="14"/>
+      <c r="N122" s="14" t="s">
+        <v>627</v>
+      </c>
+      <c r="O122" s="14" t="s">
+        <v>625</v>
+      </c>
+      <c r="P122" s="14" t="s">
+        <v>510</v>
+      </c>
+      <c r="Q122" s="14" t="s">
+        <v>492</v>
+      </c>
     </row>
     <row r="123" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A123" s="5" t="s">
@@ -9041,10 +9229,18 @@
       <c r="M123" s="15" t="s">
         <v>277</v>
       </c>
-      <c r="N123" s="14"/>
-      <c r="O123" s="14"/>
-      <c r="P123" s="14"/>
-      <c r="Q123" s="14"/>
+      <c r="N123" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="O123" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="P123" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q123" s="14" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="124" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A124" s="5" t="s">
@@ -9086,10 +9282,18 @@
       <c r="M124" s="15" t="s">
         <v>142</v>
       </c>
-      <c r="N124" s="14"/>
-      <c r="O124" s="14"/>
-      <c r="P124" s="14"/>
-      <c r="Q124" s="14"/>
+      <c r="N124" s="14" t="s">
+        <v>172</v>
+      </c>
+      <c r="O124" s="14" t="s">
+        <v>582</v>
+      </c>
+      <c r="P124" s="14" t="s">
+        <v>639</v>
+      </c>
+      <c r="Q124" s="14" t="s">
+        <v>641</v>
+      </c>
     </row>
     <row r="125" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A125" s="5" t="s">
@@ -9131,10 +9335,18 @@
       <c r="M125" s="15" t="s">
         <v>533</v>
       </c>
-      <c r="N125" s="14"/>
-      <c r="O125" s="14"/>
-      <c r="P125" s="14"/>
-      <c r="Q125" s="14"/>
+      <c r="N125" s="14" t="s">
+        <v>114</v>
+      </c>
+      <c r="O125" s="14" t="s">
+        <v>111</v>
+      </c>
+      <c r="P125" s="14" t="s">
+        <v>101</v>
+      </c>
+      <c r="Q125" s="14" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="126" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A126" s="5" t="s">
@@ -9176,10 +9388,18 @@
       <c r="M126" s="15" t="s">
         <v>169</v>
       </c>
-      <c r="N126" s="14"/>
-      <c r="O126" s="14"/>
-      <c r="P126" s="14"/>
-      <c r="Q126" s="14"/>
+      <c r="N126" s="14" t="s">
+        <v>322</v>
+      </c>
+      <c r="O126" s="14" t="s">
+        <v>282</v>
+      </c>
+      <c r="P126" s="14" t="s">
+        <v>529</v>
+      </c>
+      <c r="Q126" s="14" t="s">
+        <v>642</v>
+      </c>
     </row>
     <row r="127" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A127" s="5" t="s">
@@ -9221,10 +9441,18 @@
       <c r="M127" s="15" t="s">
         <v>83</v>
       </c>
-      <c r="N127" s="14"/>
-      <c r="O127" s="14"/>
-      <c r="P127" s="14"/>
-      <c r="Q127" s="14"/>
+      <c r="N127" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="O127" s="14" t="s">
+        <v>259</v>
+      </c>
+      <c r="P127" s="14" t="s">
+        <v>101</v>
+      </c>
+      <c r="Q127" s="14" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="128" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A128" s="5" t="s">
@@ -9266,10 +9494,18 @@
       <c r="M128" s="15" t="s">
         <v>214</v>
       </c>
-      <c r="N128" s="14"/>
-      <c r="O128" s="14"/>
-      <c r="P128" s="14"/>
-      <c r="Q128" s="14"/>
+      <c r="N128" s="14" t="s">
+        <v>628</v>
+      </c>
+      <c r="O128" s="14" t="s">
+        <v>537</v>
+      </c>
+      <c r="P128" s="14" t="s">
+        <v>312</v>
+      </c>
+      <c r="Q128" s="14" t="s">
+        <v>272</v>
+      </c>
     </row>
     <row r="129" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A129" s="5" t="s">
@@ -9311,10 +9547,18 @@
       <c r="M129" s="14" t="s">
         <v>266</v>
       </c>
-      <c r="N129" s="14"/>
-      <c r="O129" s="14"/>
-      <c r="P129" s="14"/>
-      <c r="Q129" s="14"/>
+      <c r="N129" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="O129" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="P129" s="14" t="s">
+        <v>111</v>
+      </c>
+      <c r="Q129" s="14" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="130" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A130" s="5" t="s">
@@ -9356,10 +9600,18 @@
       <c r="M130" s="14" t="s">
         <v>609</v>
       </c>
-      <c r="N130" s="14"/>
-      <c r="O130" s="14"/>
-      <c r="P130" s="14"/>
-      <c r="Q130" s="14"/>
+      <c r="N130" s="14" t="s">
+        <v>629</v>
+      </c>
+      <c r="O130" s="14" t="s">
+        <v>626</v>
+      </c>
+      <c r="P130" s="14" t="s">
+        <v>464</v>
+      </c>
+      <c r="Q130" s="14" t="s">
+        <v>461</v>
+      </c>
     </row>
     <row r="131" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A131" s="5" t="s">
@@ -9401,10 +9653,18 @@
       <c r="M131" s="14" t="s">
         <v>533</v>
       </c>
-      <c r="N131" s="14"/>
-      <c r="O131" s="14"/>
-      <c r="P131" s="14"/>
-      <c r="Q131" s="14"/>
+      <c r="N131" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="O131" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="P131" s="14" t="s">
+        <v>259</v>
+      </c>
+      <c r="Q131" s="14" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="132" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A132" s="5" t="s">
@@ -9446,10 +9706,18 @@
       <c r="M132" s="14" t="s">
         <v>125</v>
       </c>
-      <c r="N132" s="14"/>
-      <c r="O132" s="14"/>
-      <c r="P132" s="14"/>
-      <c r="Q132" s="14"/>
+      <c r="N132" s="14" t="s">
+        <v>614</v>
+      </c>
+      <c r="O132" s="14" t="s">
+        <v>161</v>
+      </c>
+      <c r="P132" s="14" t="s">
+        <v>640</v>
+      </c>
+      <c r="Q132" s="14" t="s">
+        <v>220</v>
+      </c>
     </row>
     <row r="133" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A133" s="5" t="s">
@@ -9491,10 +9759,18 @@
       <c r="M133" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="N133" s="14"/>
-      <c r="O133" s="14"/>
-      <c r="P133" s="14"/>
-      <c r="Q133" s="14"/>
+      <c r="N133" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="O133" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="P133" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q133" s="14" t="s">
+        <v>152</v>
+      </c>
     </row>
     <row r="134" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A134" s="5" t="s">

</xml_diff>